<commit_message>
fix migration and finish seeder
</commit_message>
<xml_diff>
--- a/public/excel/DB.xlsx
+++ b/public/excel/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macpro/Documents/Programming/nuramotor/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D17E898-8300-1D4C-A477-86ED14A29D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22536EC-F36D-EA49-9DDD-CA84712B4179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{02295F79-E7DE-F947-BC98-AFCC3533C3E5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>NURAMOTOR</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>change_received</t>
-  </si>
-  <si>
-    <t>type_id</t>
   </si>
   <si>
     <t>transaction_type</t>
@@ -143,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -254,11 +251,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -275,6 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,7 +654,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
@@ -658,7 +665,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
@@ -668,7 +675,9 @@
       <c r="F8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
@@ -688,8 +697,8 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="F11" s="5" t="s">
-        <v>22</v>
+      <c r="F11" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -698,9 +707,7 @@
       <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="F12" s="10"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
@@ -742,7 +749,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
@@ -763,7 +770,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>21</v>
@@ -772,16 +779,16 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>

</xml_diff>